<commit_message>
fix error in closing things
</commit_message>
<xml_diff>
--- a/docs/trainings/Training_Schedule.xlsx
+++ b/docs/trainings/Training_Schedule.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\martech_final_inspection\docs\trainings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71CC1BD0-1E65-486C-BECD-45984FFC066B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15DB4C9B-DADA-46C0-AE74-AE3B0C901873}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="PRODUCCION" sheetId="1" r:id="rId1"/>
+    <sheet name="CALIDAD" sheetId="2" r:id="rId2"/>
+    <sheet name="Usuarios" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="70">
   <si>
     <t>ENTRENAMIENTOS FINAL INSPECTION</t>
   </si>
@@ -142,13 +144,106 @@
   </si>
   <si>
     <t>1:30-1:45</t>
+  </si>
+  <si>
+    <t>8:00 - 8:20</t>
+  </si>
+  <si>
+    <t>Supervisores Calidad</t>
+  </si>
+  <si>
+    <t>PLANTA 1</t>
+  </si>
+  <si>
+    <t>PLANTA 2</t>
+  </si>
+  <si>
+    <t>PLANTA 3</t>
+  </si>
+  <si>
+    <t>Turno Primero</t>
+  </si>
+  <si>
+    <t>Turno Segundo</t>
+  </si>
+  <si>
+    <t>Turno Tercero</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-Paty Mendez, </t>
+  </si>
+  <si>
+    <t>P2-Imelda Alejandre,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> P3-Cristina Aceves</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P1-Erika Morales, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">P2-Raquel Marcial, </t>
+  </si>
+  <si>
+    <t>P3-Jose Apodaca</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P1-Laura Aguilar (Lider), </t>
+  </si>
+  <si>
+    <t xml:space="preserve">P2-Sandra Ceballos, </t>
+  </si>
+  <si>
+    <t>P3-Maricela Aceves</t>
+  </si>
+  <si>
+    <t>QC</t>
+  </si>
+  <si>
+    <t>Moldeo</t>
+  </si>
+  <si>
+    <t>PATRICIA MENDEZ</t>
+  </si>
+  <si>
+    <t>P. Méndez</t>
+  </si>
+  <si>
+    <t>gfigueroa</t>
+  </si>
+  <si>
+    <t>USUARIO</t>
+  </si>
+  <si>
+    <t>GRISELDA FIGUEROA</t>
+  </si>
+  <si>
+    <t>G.Figueroa</t>
+  </si>
+  <si>
+    <t>Leodegaria Dominguez</t>
+  </si>
+  <si>
+    <t>L.Dominguez</t>
+  </si>
+  <si>
+    <t>7 Julio 9:40</t>
+  </si>
+  <si>
+    <t>7 Julio 17:00 Hrs</t>
+  </si>
+  <si>
+    <t>7 Julio 16:00 Hrs</t>
+  </si>
+  <si>
+    <t>14:00 hrs 7 Julio</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -156,13 +251,49 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -174,15 +305,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="20" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -461,10 +600,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:F28"/>
+  <dimension ref="A3:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -474,6 +613,7 @@
     <col min="3" max="3" width="6.90625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31.1796875" customWidth="1"/>
     <col min="5" max="6" width="14.453125" customWidth="1"/>
+    <col min="7" max="7" width="12.26953125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -492,47 +632,52 @@
       <c r="E3" s="1">
         <v>44746</v>
       </c>
-      <c r="F3" s="1"/>
+      <c r="F3" s="1">
+        <v>44747</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E4" t="s">
+      <c r="D4" s="2"/>
+      <c r="E4" s="2" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E5" t="s">
+      <c r="D5" s="2"/>
+      <c r="E5" s="2" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E6" t="s">
+      <c r="D6" s="2"/>
+      <c r="E6" s="2" t="s">
         <v>31</v>
       </c>
     </row>
@@ -558,18 +703,67 @@
         <v>11</v>
       </c>
     </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
+      <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B14" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" t="s">
+      <c r="B14" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E14" t="s">
-        <v>34</v>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
@@ -577,13 +771,10 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C15" t="s">
-        <v>5</v>
-      </c>
-      <c r="E15" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
@@ -591,13 +782,10 @@
         <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C16" t="s">
-        <v>5</v>
-      </c>
-      <c r="E16" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
@@ -605,13 +793,10 @@
         <v>13</v>
       </c>
       <c r="B17" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C17" t="s">
-        <v>5</v>
-      </c>
-      <c r="E17" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
@@ -619,106 +804,78 @@
         <v>13</v>
       </c>
       <c r="B18" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" s="2"/>
+      <c r="E21" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22" s="2"/>
+      <c r="E22" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A23" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" s="2"/>
+      <c r="E23" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24" s="5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>13</v>
-      </c>
-      <c r="B19" t="s">
-        <v>19</v>
-      </c>
-      <c r="C19" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>13</v>
-      </c>
-      <c r="B20" t="s">
-        <v>20</v>
-      </c>
-      <c r="C20" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>13</v>
-      </c>
-      <c r="B21" t="s">
-        <v>22</v>
-      </c>
-      <c r="C21" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
-        <v>23</v>
-      </c>
-      <c r="B24" t="s">
-        <v>24</v>
-      </c>
-      <c r="C24" t="s">
-        <v>5</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>35</v>
-      </c>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C25" t="s">
-        <v>5</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>23</v>
-      </c>
-      <c r="B26" t="s">
-        <v>26</v>
-      </c>
-      <c r="C26" t="s">
-        <v>5</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
-        <v>23</v>
-      </c>
-      <c r="B27" t="s">
-        <v>27</v>
-      </c>
-      <c r="C27" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>23</v>
-      </c>
-      <c r="B28" t="s">
-        <v>28</v>
-      </c>
-      <c r="C28" t="s">
         <v>11</v>
       </c>
     </row>
@@ -726,4 +883,169 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE4FC1EC-A0D9-4037-B053-3DFF0970AD7D}">
+  <dimension ref="B2:H5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="24.08984375" customWidth="1"/>
+    <col min="3" max="3" width="21.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.36328125" customWidth="1"/>
+    <col min="5" max="5" width="18.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.26953125" customWidth="1"/>
+    <col min="7" max="7" width="20.6328125" customWidth="1"/>
+    <col min="8" max="8" width="14.54296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E5" t="s">
+        <v>54</v>
+      </c>
+      <c r="G5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{134C6E17-500F-4D2A-8550-8732E257E674}">
+  <dimension ref="B3:G7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="20.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.54296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B5">
+        <v>17343</v>
+      </c>
+      <c r="C5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B6">
+        <v>31034</v>
+      </c>
+      <c r="C6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D6" t="s">
+        <v>63</v>
+      </c>
+      <c r="F6" t="s">
+        <v>60</v>
+      </c>
+      <c r="G6">
+        <v>123456</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B7">
+        <v>8666</v>
+      </c>
+      <c r="C7" t="s">
+        <v>64</v>
+      </c>
+      <c r="D7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>